<commit_message>
Updated IR sensor data spreadsheet
</commit_message>
<xml_diff>
--- a/Resources/IR Sensor Data.xlsx
+++ b/Resources/IR Sensor Data.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="7635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="7635" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Short Range" sheetId="2" r:id="rId1"/>
     <sheet name="Medium Range" sheetId="3" r:id="rId2"/>
     <sheet name="Older Short Range Samples" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>White Surface</t>
   </si>
@@ -139,12 +135,15 @@
   <si>
     <t>Averages</t>
   </si>
+  <si>
+    <t>reading</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,18 +232,308 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Medium Range'!$M$6:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>536.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>493.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>375.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>337.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>321.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>272.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>262.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>252.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>245.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>182</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Medium Range'!$N$6:$N$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>370</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="82915712"/>
+        <c:axId val="82917248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="82915712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82917248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="82917248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82915712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -273,10 +562,12 @@
         </a:p>
       </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -317,12 +608,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.4903636348861965"/>
-                  <c:y val="-0.74671977556501146"/>
+                  <c:y val="-0.74671977556501223"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -529,15 +821,25 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="89302912"/>
-        <c:axId val="89304448"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="82950784"/>
+        <c:axId val="84427136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89302912"/>
+        <c:axId val="82950784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -555,6 +857,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -589,15 +892,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89304448"/>
+        <c:crossAx val="84427136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89304448"/>
+        <c:axId val="84427136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -615,6 +919,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -649,7 +954,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89302912"/>
+        <c:crossAx val="82950784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -663,6 +968,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -691,13 +997,597 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.37922468734699694"/>
+                  <c:y val="0.10082276173811609"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="1">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="12700"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="3175"/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.37326356080489942"/>
+                  <c:y val="-2.8135753864100325E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$5:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="1">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="84490880"/>
+        <c:axId val="84496768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="84490880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84496768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="84496768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84490880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -711,6 +1601,41 @@
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -994,19 +1919,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1014,7 +1939,7 @@
         <v>41479</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1028,7 +1953,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>535</v>
       </c>
@@ -1039,7 +1964,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>460</v>
       </c>
@@ -1050,7 +1975,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>405</v>
       </c>
@@ -1061,7 +1986,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>355</v>
       </c>
@@ -1072,7 +1997,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>315</v>
       </c>
@@ -1083,7 +2008,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>285</v>
       </c>
@@ -1094,7 +2019,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>260</v>
       </c>
@@ -1105,7 +2030,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>237</v>
       </c>
@@ -1116,7 +2041,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>222</v>
       </c>
@@ -1127,7 +2052,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>210</v>
       </c>
@@ -1138,7 +2063,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>200</v>
       </c>
@@ -1149,7 +2074,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>190</v>
       </c>
@@ -1160,7 +2085,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>180</v>
       </c>
@@ -1171,7 +2096,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>170</v>
       </c>
@@ -1182,7 +2107,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>160</v>
       </c>
@@ -1193,7 +2118,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>157</v>
       </c>
@@ -1204,7 +2129,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>150</v>
       </c>
@@ -1215,7 +2140,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>140</v>
       </c>
@@ -1226,7 +2151,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>135</v>
       </c>
@@ -1237,7 +2162,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>132</v>
       </c>
@@ -1248,7 +2173,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>127</v>
       </c>
@@ -1259,7 +2184,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>125</v>
       </c>
@@ -1270,7 +2195,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>122</v>
       </c>
@@ -1281,7 +2206,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>120</v>
       </c>
@@ -1292,232 +2217,232 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>310</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>330</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>340</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="5:5">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>360</v>
       </c>
     </row>
-    <row r="34" spans="5:5">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>370</v>
       </c>
     </row>
-    <row r="35" spans="5:5">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>380</v>
       </c>
     </row>
-    <row r="36" spans="5:5">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>390</v>
       </c>
     </row>
-    <row r="37" spans="5:5">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>400</v>
       </c>
     </row>
-    <row r="38" spans="5:5">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>410</v>
       </c>
     </row>
-    <row r="39" spans="5:5">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>420</v>
       </c>
     </row>
-    <row r="40" spans="5:5">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>430</v>
       </c>
     </row>
-    <row r="41" spans="5:5">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>440</v>
       </c>
     </row>
-    <row r="42" spans="5:5">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E42">
         <v>450</v>
       </c>
     </row>
-    <row r="43" spans="5:5">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>460</v>
       </c>
     </row>
-    <row r="44" spans="5:5">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>470</v>
       </c>
     </row>
-    <row r="45" spans="5:5">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E45">
         <v>480</v>
       </c>
     </row>
-    <row r="46" spans="5:5">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E46">
         <v>490</v>
       </c>
     </row>
-    <row r="47" spans="5:5">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E47">
         <v>500</v>
       </c>
     </row>
-    <row r="48" spans="5:5">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>510</v>
       </c>
     </row>
-    <row r="49" spans="5:5">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E49">
         <v>520</v>
       </c>
     </row>
-    <row r="50" spans="5:5">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E50">
         <v>530</v>
       </c>
     </row>
-    <row r="51" spans="5:5">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E51">
         <v>540</v>
       </c>
     </row>
-    <row r="52" spans="5:5">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E52">
         <v>550</v>
       </c>
     </row>
-    <row r="53" spans="5:5">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E53">
         <v>560</v>
       </c>
     </row>
-    <row r="54" spans="5:5">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E54">
         <v>570</v>
       </c>
     </row>
-    <row r="55" spans="5:5">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E55">
         <v>580</v>
       </c>
     </row>
-    <row r="56" spans="5:5">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E56">
         <v>590</v>
       </c>
     </row>
-    <row r="57" spans="5:5">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E57">
         <v>600</v>
       </c>
     </row>
-    <row r="58" spans="5:5">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E58">
         <v>610</v>
       </c>
     </row>
-    <row r="59" spans="5:5">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E59">
         <v>620</v>
       </c>
     </row>
-    <row r="60" spans="5:5">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E60">
         <v>630</v>
       </c>
     </row>
-    <row r="61" spans="5:5">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E61">
         <v>640</v>
       </c>
     </row>
-    <row r="62" spans="5:5">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E62">
         <v>650</v>
       </c>
     </row>
-    <row r="63" spans="5:5">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E63">
         <v>660</v>
       </c>
     </row>
-    <row r="64" spans="5:5">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E64">
         <v>670</v>
       </c>
     </row>
-    <row r="65" spans="5:5">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65">
         <v>680</v>
       </c>
     </row>
-    <row r="66" spans="5:5">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66">
         <v>690</v>
       </c>
     </row>
-    <row r="67" spans="5:5">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E67">
         <v>700</v>
       </c>
     </row>
-    <row r="68" spans="5:5">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E68">
         <v>710</v>
       </c>
     </row>
-    <row r="69" spans="5:5">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E69">
         <v>720</v>
       </c>
     </row>
-    <row r="70" spans="5:5">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70">
         <v>730</v>
       </c>
     </row>
-    <row r="71" spans="5:5">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71">
         <v>740</v>
       </c>
     </row>
-    <row r="72" spans="5:5">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E72">
         <v>750</v>
       </c>
@@ -1528,21 +2453,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M72"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1553,7 +2478,7 @@
         <v>41479</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1585,7 +2510,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>637</v>
       </c>
@@ -1605,7 +2530,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>620</v>
       </c>
@@ -1616,7 +2541,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>565</v>
       </c>
@@ -1627,7 +2552,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>520</v>
       </c>
@@ -1650,8 +2575,11 @@
         <f>AVERAGE(J6,K6,L6)</f>
         <v>575</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>475</v>
       </c>
@@ -1683,8 +2611,11 @@
         <f t="shared" ref="M7:M34" si="0">AVERAGE(J7,K7,L7)</f>
         <v>536.66666666666663</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>442</v>
       </c>
@@ -1707,8 +2638,11 @@
         <f t="shared" si="0"/>
         <v>493.33333333333331</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>412</v>
       </c>
@@ -1731,8 +2665,11 @@
         <f t="shared" si="0"/>
         <v>455</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>385</v>
       </c>
@@ -1755,8 +2692,11 @@
         <f t="shared" si="0"/>
         <v>426</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>362</v>
       </c>
@@ -1779,8 +2719,11 @@
         <f t="shared" si="0"/>
         <v>399</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>339</v>
       </c>
@@ -1803,8 +2746,11 @@
         <f t="shared" si="0"/>
         <v>375.66666666666669</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>323</v>
       </c>
@@ -1827,8 +2773,11 @@
         <f t="shared" si="0"/>
         <v>357</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>304</v>
       </c>
@@ -1851,8 +2800,11 @@
         <f t="shared" si="0"/>
         <v>337.33333333333331</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>293</v>
       </c>
@@ -1875,8 +2827,11 @@
         <f t="shared" si="0"/>
         <v>321.66666666666669</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>280</v>
       </c>
@@ -1899,8 +2854,11 @@
         <f t="shared" si="0"/>
         <v>305</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>268</v>
       </c>
@@ -1932,8 +2890,11 @@
         <f t="shared" si="0"/>
         <v>295</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>258</v>
       </c>
@@ -1956,8 +2917,11 @@
         <f t="shared" si="0"/>
         <v>285</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>249</v>
       </c>
@@ -1977,8 +2941,11 @@
         <f t="shared" si="0"/>
         <v>272.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>237</v>
       </c>
@@ -1998,8 +2965,11 @@
         <f t="shared" si="0"/>
         <v>262.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>229</v>
       </c>
@@ -2019,8 +2989,11 @@
         <f t="shared" si="0"/>
         <v>252.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>221</v>
       </c>
@@ -2043,8 +3016,11 @@
         <f t="shared" si="0"/>
         <v>245.66666666666666</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>212</v>
       </c>
@@ -2064,8 +3040,11 @@
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>204</v>
       </c>
@@ -2085,8 +3064,11 @@
         <f t="shared" si="0"/>
         <v>233</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>196</v>
       </c>
@@ -2106,8 +3088,11 @@
         <f t="shared" si="0"/>
         <v>227</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>192</v>
       </c>
@@ -2127,8 +3112,11 @@
         <f t="shared" si="0"/>
         <v>224</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>184</v>
       </c>
@@ -2160,8 +3148,11 @@
         <f t="shared" si="0"/>
         <v>218</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>178</v>
       </c>
@@ -2181,8 +3172,11 @@
         <f t="shared" si="0"/>
         <v>214</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>173</v>
       </c>
@@ -2202,8 +3196,11 @@
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>168</v>
       </c>
@@ -2223,8 +3220,11 @@
         <f t="shared" si="0"/>
         <v>203</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>164</v>
       </c>
@@ -2241,8 +3241,11 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>158</v>
       </c>
@@ -2259,8 +3262,11 @@
         <f t="shared" si="0"/>
         <v>197</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>152</v>
       </c>
@@ -2277,8 +3283,11 @@
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>149</v>
       </c>
@@ -2295,8 +3304,11 @@
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>145</v>
       </c>
@@ -2307,7 +3319,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>141</v>
       </c>
@@ -2318,7 +3330,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>139</v>
       </c>
@@ -2338,7 +3350,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>134</v>
       </c>
@@ -2349,7 +3361,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>130</v>
       </c>
@@ -2360,7 +3372,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>128</v>
       </c>
@@ -2371,7 +3383,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>125</v>
       </c>
@@ -2382,7 +3394,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>122</v>
       </c>
@@ -2393,7 +3405,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>118</v>
       </c>
@@ -2404,7 +3416,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>115</v>
       </c>
@@ -2415,7 +3427,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>114</v>
       </c>
@@ -2426,7 +3438,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>111</v>
       </c>
@@ -2437,7 +3449,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>109</v>
       </c>
@@ -2457,7 +3469,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>107</v>
       </c>
@@ -2468,7 +3480,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>103</v>
       </c>
@@ -2479,7 +3491,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>100</v>
       </c>
@@ -2490,7 +3502,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>98</v>
       </c>
@@ -2501,7 +3513,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>98</v>
       </c>
@@ -2512,7 +3524,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>98</v>
       </c>
@@ -2523,7 +3535,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>96</v>
       </c>
@@ -2534,7 +3546,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>94</v>
       </c>
@@ -2545,7 +3557,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>94</v>
       </c>
@@ -2556,7 +3568,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>92</v>
       </c>
@@ -2576,7 +3588,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>88</v>
       </c>
@@ -2587,7 +3599,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>86</v>
       </c>
@@ -2598,7 +3610,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>630</v>
       </c>
@@ -2606,7 +3618,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>640</v>
       </c>
@@ -2614,7 +3626,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>650</v>
       </c>
@@ -2622,7 +3634,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>660</v>
       </c>
@@ -2630,7 +3642,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>670</v>
       </c>
@@ -2638,7 +3650,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>680</v>
       </c>
@@ -2646,7 +3658,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>690</v>
       </c>
@@ -2654,7 +3666,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>79</v>
       </c>
@@ -2674,7 +3686,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>710</v>
       </c>
@@ -2682,7 +3694,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>720</v>
       </c>
@@ -2690,7 +3702,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>730</v>
       </c>
@@ -2698,7 +3710,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>740</v>
       </c>
@@ -2706,7 +3718,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>750</v>
       </c>
@@ -2716,18 +3728,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
@@ -2737,7 +3750,7 @@
     <col min="7" max="7" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="8" t="s">
         <v>8</v>
@@ -2748,7 +3761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -2760,7 +3773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -2782,7 +3795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>5</v>
       </c>
@@ -2809,7 +3822,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>6</v>
       </c>
@@ -2836,7 +3849,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>7</v>
       </c>
@@ -2863,7 +3876,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>8</v>
       </c>
@@ -2890,7 +3903,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>9</v>
       </c>
@@ -2915,7 +3928,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>10</v>
       </c>
@@ -2945,7 +3958,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>11</v>
       </c>
@@ -2975,7 +3988,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>12</v>
       </c>
@@ -3003,7 +4016,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>13</v>
       </c>
@@ -3031,7 +4044,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>14</v>
       </c>
@@ -3059,7 +4072,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>15</v>
       </c>
@@ -3082,7 +4095,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>16</v>
       </c>
@@ -3107,7 +4120,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.25">
+    <row r="16" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>17</v>
       </c>
@@ -3132,7 +4145,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>18</v>
       </c>
@@ -3154,7 +4167,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>19</v>
       </c>
@@ -3176,7 +4189,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>20</v>
       </c>
@@ -3198,7 +4211,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>21</v>
       </c>
@@ -3220,7 +4233,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>22</v>
       </c>
@@ -3242,7 +4255,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>23</v>
       </c>
@@ -3264,7 +4277,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>24</v>
       </c>
@@ -3286,7 +4299,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>25</v>
       </c>
@@ -3308,7 +4321,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>26</v>
       </c>
@@ -3330,7 +4343,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>27</v>
       </c>
@@ -3352,7 +4365,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>28</v>
       </c>
@@ -3374,7 +4387,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>29</v>
       </c>
@@ -3396,7 +4409,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>30</v>
       </c>
@@ -3429,4 +4442,813 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>627</v>
+      </c>
+      <c r="F2">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>70</v>
+      </c>
+      <c r="D3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>479</v>
+      </c>
+      <c r="F6">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>110</v>
+      </c>
+      <c r="D7">
+        <v>110</v>
+      </c>
+      <c r="E7">
+        <v>445</v>
+      </c>
+      <c r="F7">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="D8">
+        <v>120</v>
+      </c>
+      <c r="E8">
+        <v>413</v>
+      </c>
+      <c r="F8">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>130</v>
+      </c>
+      <c r="D9">
+        <v>130</v>
+      </c>
+      <c r="E9">
+        <v>386</v>
+      </c>
+      <c r="F9">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>140</v>
+      </c>
+      <c r="D10">
+        <v>140</v>
+      </c>
+      <c r="E10">
+        <v>360</v>
+      </c>
+      <c r="F10">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>150</v>
+      </c>
+      <c r="D11">
+        <v>150</v>
+      </c>
+      <c r="E11">
+        <v>337</v>
+      </c>
+      <c r="F11">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>160</v>
+      </c>
+      <c r="D12">
+        <v>160</v>
+      </c>
+      <c r="E12">
+        <v>321</v>
+      </c>
+      <c r="F12">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>170</v>
+      </c>
+      <c r="D13">
+        <v>170</v>
+      </c>
+      <c r="E13">
+        <v>302</v>
+      </c>
+      <c r="F13">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>180</v>
+      </c>
+      <c r="D14">
+        <v>180</v>
+      </c>
+      <c r="E14">
+        <v>287</v>
+      </c>
+      <c r="F14">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>190</v>
+      </c>
+      <c r="D15">
+        <v>190</v>
+      </c>
+      <c r="E15">
+        <v>271</v>
+      </c>
+      <c r="F15">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>200</v>
+      </c>
+      <c r="D16">
+        <v>200</v>
+      </c>
+      <c r="E16">
+        <v>263</v>
+      </c>
+      <c r="F16">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>210</v>
+      </c>
+      <c r="D17">
+        <v>210</v>
+      </c>
+      <c r="E17">
+        <v>251</v>
+      </c>
+      <c r="F17">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>220</v>
+      </c>
+      <c r="D18">
+        <v>220</v>
+      </c>
+      <c r="E18">
+        <v>239</v>
+      </c>
+      <c r="F18">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>230</v>
+      </c>
+      <c r="D19">
+        <v>230</v>
+      </c>
+      <c r="E19">
+        <v>231</v>
+      </c>
+      <c r="F19">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>240</v>
+      </c>
+      <c r="D20">
+        <v>240</v>
+      </c>
+      <c r="E20">
+        <v>223</v>
+      </c>
+      <c r="F20">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>250</v>
+      </c>
+      <c r="D21">
+        <v>250</v>
+      </c>
+      <c r="E21">
+        <v>215</v>
+      </c>
+      <c r="F21">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>260</v>
+      </c>
+      <c r="D22">
+        <v>260</v>
+      </c>
+      <c r="E22">
+        <v>208</v>
+      </c>
+      <c r="F22">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>270</v>
+      </c>
+      <c r="D23">
+        <v>270</v>
+      </c>
+      <c r="E23">
+        <v>203</v>
+      </c>
+      <c r="F23">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>280</v>
+      </c>
+      <c r="D24">
+        <v>280</v>
+      </c>
+      <c r="E24">
+        <v>195</v>
+      </c>
+      <c r="F24">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>290</v>
+      </c>
+      <c r="D25">
+        <v>290</v>
+      </c>
+      <c r="E25">
+        <v>191</v>
+      </c>
+      <c r="F25">
+        <v>186</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>300</v>
+      </c>
+      <c r="D26">
+        <v>300</v>
+      </c>
+      <c r="E26">
+        <v>187</v>
+      </c>
+      <c r="F26">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>310</v>
+      </c>
+      <c r="D27">
+        <v>310</v>
+      </c>
+      <c r="E27">
+        <v>183</v>
+      </c>
+      <c r="F27">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>320</v>
+      </c>
+      <c r="D28">
+        <v>320</v>
+      </c>
+      <c r="E28">
+        <v>179</v>
+      </c>
+      <c r="F28">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>330</v>
+      </c>
+      <c r="D29">
+        <v>330</v>
+      </c>
+      <c r="E29">
+        <v>175</v>
+      </c>
+      <c r="F29">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>340</v>
+      </c>
+      <c r="D30">
+        <v>340</v>
+      </c>
+      <c r="E30">
+        <v>171</v>
+      </c>
+      <c r="F30">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>350</v>
+      </c>
+      <c r="D31">
+        <v>350</v>
+      </c>
+      <c r="E31">
+        <v>167</v>
+      </c>
+      <c r="F31">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>360</v>
+      </c>
+      <c r="D32">
+        <v>360</v>
+      </c>
+      <c r="E32">
+        <v>163</v>
+      </c>
+      <c r="F32">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>370</v>
+      </c>
+      <c r="D33">
+        <v>370</v>
+      </c>
+      <c r="E33">
+        <v>159</v>
+      </c>
+      <c r="F33">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>380</v>
+      </c>
+      <c r="D34">
+        <v>380</v>
+      </c>
+      <c r="E34">
+        <v>155</v>
+      </c>
+      <c r="F34">
+        <v>150</v>
+      </c>
+      <c r="H34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>390</v>
+      </c>
+      <c r="D35">
+        <v>390</v>
+      </c>
+      <c r="E35">
+        <v>151</v>
+      </c>
+      <c r="F35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>400</v>
+      </c>
+      <c r="D36">
+        <v>400</v>
+      </c>
+      <c r="E36">
+        <v>151</v>
+      </c>
+      <c r="F36">
+        <v>142</v>
+      </c>
+      <c r="I36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>410</v>
+      </c>
+      <c r="D37">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>420</v>
+      </c>
+      <c r="D38">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>430</v>
+      </c>
+      <c r="D39">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>440</v>
+      </c>
+      <c r="D40">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>450</v>
+      </c>
+      <c r="D41">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>460</v>
+      </c>
+      <c r="D42">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>470</v>
+      </c>
+      <c r="D43">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>480</v>
+      </c>
+      <c r="D44">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>490</v>
+      </c>
+      <c r="D45">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>500</v>
+      </c>
+      <c r="D46">
+        <v>500</v>
+      </c>
+      <c r="E46">
+        <v>142</v>
+      </c>
+      <c r="F46">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>510</v>
+      </c>
+      <c r="D47">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>520</v>
+      </c>
+      <c r="D48">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>530</v>
+      </c>
+      <c r="D49">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>540</v>
+      </c>
+      <c r="D50">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>550</v>
+      </c>
+      <c r="D51">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>560</v>
+      </c>
+      <c r="D52">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>570</v>
+      </c>
+      <c r="D53">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>580</v>
+      </c>
+      <c r="D54">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>590</v>
+      </c>
+      <c r="D55">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>600</v>
+      </c>
+      <c r="D56">
+        <v>600</v>
+      </c>
+      <c r="E56">
+        <v>134</v>
+      </c>
+      <c r="F56">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>610</v>
+      </c>
+      <c r="D57">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>620</v>
+      </c>
+      <c r="D58">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>630</v>
+      </c>
+      <c r="D59">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>640</v>
+      </c>
+      <c r="D60">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>650</v>
+      </c>
+      <c r="D61">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>660</v>
+      </c>
+      <c r="D62">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>670</v>
+      </c>
+      <c r="D63">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>680</v>
+      </c>
+      <c r="D64">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>690</v>
+      </c>
+      <c r="D65">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>700</v>
+      </c>
+      <c r="D66">
+        <v>700</v>
+      </c>
+      <c r="E66">
+        <v>136</v>
+      </c>
+      <c r="F66">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>710</v>
+      </c>
+      <c r="D67">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>720</v>
+      </c>
+      <c r="D68">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>730</v>
+      </c>
+      <c r="D69">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>740</v>
+      </c>
+      <c r="D70">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>750</v>
+      </c>
+      <c r="D71">
+        <v>750</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Altered IR mm calculations
Uncommented GridNav virtualisation lines.
</commit_message>
<xml_diff>
--- a/Resources/IR Sensor Data.xlsx
+++ b/Resources/IR Sensor Data.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="7635" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="7635"/>
   </bookViews>
   <sheets>
-    <sheet name="Short Range" sheetId="2" r:id="rId1"/>
-    <sheet name="Medium Range" sheetId="3" r:id="rId2"/>
-    <sheet name="Older Short Range Samples" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1 (2)" sheetId="5" r:id="rId1"/>
+    <sheet name="Short Range" sheetId="2" r:id="rId2"/>
+    <sheet name="Medium Range" sheetId="3" r:id="rId3"/>
+    <sheet name="Older Short Range Samples" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>White Surface</t>
   </si>
@@ -259,201 +260,89 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+          </c:marker>
           <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="4"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.37922468734699694"/>
+                  <c:y val="0.10082276173811609"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Medium Range'!$M$6:$M$34</c:f>
+              <c:f>'Sheet1 (2)'!$D$5:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>575</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>536.66666666666663</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>493.33333333333331</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>455</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>426</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>399</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>375.66666666666669</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>357</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>337.33333333333331</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>321.66666666666669</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>295</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>285</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>272.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>262.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>252.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>245.66666666666666</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>233</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>182</c:v>
-                </c:pt>
+                <c:ptCount val="32"/>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Medium Range'!$N$6:$N$34</c:f>
+              <c:f>'Sheet1 (2)'!$E$5:$E$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>370</c:v>
-                </c:pt>
+                <c:ptCount val="32"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="12700"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="3175"/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.37326356080489942"/>
+                  <c:y val="-2.8135753864100325E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$D$5:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$F$5:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -467,11 +356,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82915712"/>
-        <c:axId val="82917248"/>
+        <c:axId val="60872960"/>
+        <c:axId val="62922752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82915712"/>
+        <c:axId val="60872960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,12 +370,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82917248"/>
+        <c:crossAx val="62922752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82917248"/>
+        <c:axId val="62922752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,13 +386,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82915712"/>
+        <c:crossAx val="60872960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -512,13 +402,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-AU"/>
@@ -831,11 +721,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82950784"/>
-        <c:axId val="84427136"/>
+        <c:axId val="64093184"/>
+        <c:axId val="64123648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82950784"/>
+        <c:axId val="64093184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,12 +782,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84427136"/>
+        <c:crossAx val="64123648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84427136"/>
+        <c:axId val="64123648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,7 +844,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82950784"/>
+        <c:crossAx val="64093184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1003,7 +893,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-AU"/>
@@ -1500,11 +1390,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84490880"/>
-        <c:axId val="84496768"/>
+        <c:axId val="64502784"/>
+        <c:axId val="64508672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84490880"/>
+        <c:axId val="64502784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,12 +1404,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84496768"/>
+        <c:crossAx val="64508672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84496768"/>
+        <c:axId val="64508672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1530,7 +1420,432 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84490880"/>
+        <c:crossAx val="64502784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$3:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$3:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="68108672"/>
+        <c:axId val="68106880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="68108672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68106880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="68106880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68108672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1546,13 +1861,2217 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$29:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$29:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="40481536"/>
+        <c:axId val="87268352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="40481536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87268352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="87268352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40481536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$17:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$17:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="68235648"/>
+        <c:axId val="68229760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="68235648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68229760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="68229760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68235648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$9:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$9:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="40454400"/>
+        <c:axId val="39373440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="40454400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39373440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="39373440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40454400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$3:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>437</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="87351296"/>
+        <c:axId val="87349504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="87351296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87349504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="87349504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87351296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$6:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$6:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="68187648"/>
+        <c:axId val="68186112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="68187648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68186112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="68186112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68187648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$3:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$3:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$3:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$C$3:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>604.33000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>518.33000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>432.33000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>374.16999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>333.66999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>293.16999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>257.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>241.46400000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>225.42800000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>209.39200000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>193.35600000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>177.32000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>161.28400000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>145.24800000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>137.518</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>131.81900000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>126.12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>120.42100000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>114.72200000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>109.023</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>103.32400000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>97.625</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>91.926000000000016</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>86.227000000000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>80.527999999999992</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>74.829000000000008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>71.03</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>69.363000000000014</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>67.696000000000012</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>66.029000000000011</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>64.362000000000009</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>62.695000000000007</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>61.028000000000013</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>59.361000000000011</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>57.69400000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>56.027000000000015</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>54.360000000000014</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>52.693000000000012</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>51.02600000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>49.359000000000009</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>47.692000000000007</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>46.025000000000006</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44.358000000000018</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42.691000000000017</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>41.024000000000015</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>39.357000000000014</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>37.690000000000012</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>36.02300000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>34.356000000000009</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>32.689000000000007</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>31.02200000000002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>29.355000000000018</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>27.688000000000017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="40477824"/>
+        <c:axId val="40454016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="40477824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40454016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="40454016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40477824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Medium Range'!$M$6:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>536.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>493.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>375.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>337.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>321.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>272.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>262.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>252.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>245.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>182</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Medium Range'!$N$6:$N$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>370</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64033536"/>
+        <c:axId val="64035072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64033536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64035072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64035072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64033536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1587,7 +4106,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1622,7 +4141,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1920,6 +4439,677 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>609</v>
+      </c>
+      <c r="C3">
+        <f>-8.6*A3+948.33</f>
+        <v>604.33000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>509</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C5" si="0">-8.6*A4+948.33</f>
+        <v>518.33000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>437</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>432.33000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>375</v>
+      </c>
+      <c r="C6">
+        <f>-4.05*A6+657.67</f>
+        <v>374.16999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>332</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C8" si="1">-4.05*A7+657.67</f>
+        <v>333.66999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <v>294</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>293.16999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>267</v>
+      </c>
+      <c r="C9">
+        <f>-1.6036*A9+417.86</f>
+        <v>257.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="B10">
+        <v>243</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C16" si="2">-1.6036*A10+417.86</f>
+        <v>241.46400000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>120</v>
+      </c>
+      <c r="B11">
+        <v>220</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>225.42800000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>130</v>
+      </c>
+      <c r="B12">
+        <v>202</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>209.39200000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>140</v>
+      </c>
+      <c r="B13">
+        <v>187</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>193.35600000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>150</v>
+      </c>
+      <c r="B14">
+        <v>176</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>177.32000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>160</v>
+      </c>
+      <c r="B15">
+        <v>164</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>161.28400000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>170</v>
+      </c>
+      <c r="B16">
+        <v>152</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>145.24800000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>180</v>
+      </c>
+      <c r="B17">
+        <v>144</v>
+      </c>
+      <c r="C17">
+        <f>-0.5699*A17+240.1</f>
+        <v>137.518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>190</v>
+      </c>
+      <c r="B18">
+        <v>133</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C28" si="3">-0.5699*A18+240.1</f>
+        <v>131.81900000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>200</v>
+      </c>
+      <c r="B19">
+        <v>125</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="3"/>
+        <v>126.12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>210</v>
+      </c>
+      <c r="B20">
+        <v>119</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="3"/>
+        <v>120.42100000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>220</v>
+      </c>
+      <c r="B21">
+        <v>112</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="3"/>
+        <v>114.72200000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>230</v>
+      </c>
+      <c r="B22">
+        <v>107</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>109.023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>240</v>
+      </c>
+      <c r="B23">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>103.32400000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>250</v>
+      </c>
+      <c r="B24">
+        <v>95</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>97.625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>260</v>
+      </c>
+      <c r="B25">
+        <v>91</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>91.926000000000016</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>270</v>
+      </c>
+      <c r="B26">
+        <v>87</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>86.227000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>280</v>
+      </c>
+      <c r="B27">
+        <v>83</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>80.527999999999992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>290</v>
+      </c>
+      <c r="B28">
+        <v>79</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="3"/>
+        <v>74.829000000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>300</v>
+      </c>
+      <c r="B29">
+        <v>77</v>
+      </c>
+      <c r="C29">
+        <f>-0.1667*A29+121.04</f>
+        <v>71.03</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>310</v>
+      </c>
+      <c r="B30">
+        <v>75</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:C55" si="4">-0.1667*A30+121.04</f>
+        <v>69.363000000000014</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>320</v>
+      </c>
+      <c r="B31">
+        <v>71</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="4"/>
+        <v>67.696000000000012</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>330</v>
+      </c>
+      <c r="B32">
+        <v>66</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="4"/>
+        <v>66.029000000000011</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>340</v>
+      </c>
+      <c r="B33">
+        <v>66</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="4"/>
+        <v>64.362000000000009</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>350</v>
+      </c>
+      <c r="B34">
+        <v>62</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="4"/>
+        <v>62.695000000000007</v>
+      </c>
+      <c r="H34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>360</v>
+      </c>
+      <c r="B35">
+        <v>58</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="4"/>
+        <v>61.028000000000013</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>370</v>
+      </c>
+      <c r="B36">
+        <v>58</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="4"/>
+        <v>59.361000000000011</v>
+      </c>
+      <c r="I36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>380</v>
+      </c>
+      <c r="B37">
+        <v>54</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="4"/>
+        <v>57.69400000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>390</v>
+      </c>
+      <c r="B38">
+        <v>54</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="4"/>
+        <v>56.027000000000015</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>400</v>
+      </c>
+      <c r="B39">
+        <v>52</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="4"/>
+        <v>54.360000000000014</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>410</v>
+      </c>
+      <c r="B40">
+        <v>50</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="4"/>
+        <v>52.693000000000012</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>420</v>
+      </c>
+      <c r="B41">
+        <v>50</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="4"/>
+        <v>51.02600000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>430</v>
+      </c>
+      <c r="B42">
+        <v>46</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="4"/>
+        <v>49.359000000000009</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>440</v>
+      </c>
+      <c r="B43">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="4"/>
+        <v>47.692000000000007</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>450</v>
+      </c>
+      <c r="B44">
+        <v>46</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="4"/>
+        <v>46.025000000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>460</v>
+      </c>
+      <c r="B45">
+        <v>42</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="4"/>
+        <v>44.358000000000018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>470</v>
+      </c>
+      <c r="B46">
+        <v>42</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="4"/>
+        <v>42.691000000000017</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>480</v>
+      </c>
+      <c r="B47">
+        <v>38</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="4"/>
+        <v>41.024000000000015</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>490</v>
+      </c>
+      <c r="B48">
+        <v>38</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="4"/>
+        <v>39.357000000000014</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>500</v>
+      </c>
+      <c r="B49">
+        <v>38</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="4"/>
+        <v>37.690000000000012</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>510</v>
+      </c>
+      <c r="B50">
+        <v>36</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="4"/>
+        <v>36.02300000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>520</v>
+      </c>
+      <c r="B51">
+        <v>34</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="4"/>
+        <v>34.356000000000009</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>530</v>
+      </c>
+      <c r="B52">
+        <v>34</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="4"/>
+        <v>32.689000000000007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>540</v>
+      </c>
+      <c r="B53">
+        <v>34</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="4"/>
+        <v>31.02200000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>550</v>
+      </c>
+      <c r="B54">
+        <v>34</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="4"/>
+        <v>29.355000000000018</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>560</v>
+      </c>
+      <c r="B55">
+        <v>32</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="4"/>
+        <v>27.688000000000017</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <f>(121.04-37)/0.1667</f>
+        <v>504.13917216556695</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2452,7 +5642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N72"/>
   <sheetViews>
@@ -3732,7 +6922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -4444,12 +7634,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>